<commit_message>
new condition column in catRev1_trials files
</commit_message>
<xml_diff>
--- a/data/santTest_CatRev1_within_2024-02-18_12h51.39.739.xlsx
+++ b/data/santTest_CatRev1_within_2024-02-18_12h51.39.739.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/category_reversal/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/categoricalReversalLerning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:40009_{48BA4409-59E9-41B9-B3F3-49D922D3FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{419C06BF-81B8-43D2-8681-286BF91B218F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:40009_{48BA4409-59E9-41B9-B3F3-49D922D3FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE36D3B7-1232-4433-870C-5F1E10D8B5AB}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2160,6 +2160,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2459,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ7" workbookViewId="0">
-      <selection activeCell="CH12" sqref="CH12"/>
+    <sheetView tabSelected="1" topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="BU1" sqref="BU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3058,7 +3062,7 @@
         <v>0.375</v>
       </c>
       <c r="CO4">
-        <f t="shared" ref="CO4:CP14" si="2">AVERAGEIFS($BD$4:$BD$387,$D$4:$D$387,CO$2,$E$4:$E$387,$CI4,$P$4:$P$387,$CJ4)</f>
+        <f t="shared" ref="CO4:CO14" si="2">AVERAGEIFS($BD$4:$BD$387,$D$4:$D$387,CO$2,$E$4:$E$387,$CI4,$P$4:$P$387,$CJ4)</f>
         <v>1.0740969312464568</v>
       </c>
       <c r="CP4">

</xml_diff>